<commit_message>
Updated plots and data cleanin
</commit_message>
<xml_diff>
--- a/dataproject/imf_name_cp_lookup.xlsx
+++ b/dataproject/imf_name_cp_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c5b92eedfc9a9d5/Skrivebord/KU/8. semester/Introduction to Programming/projects-2024-mikkel-thomas/dataproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{57B5C8A0-D522-4D95-BBF0-8F0DB0F02F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65A571B2-AEAB-45BE-A9BC-C7B1CD1EBFEE}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{57B5C8A0-D522-4D95-BBF0-8F0DB0F02F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52ABE74D-5961-4680-B0FE-99A41FFA45AB}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1845" yWindow="1845" windowWidth="18525" windowHeight="10035" xr2:uid="{DB5003FB-30CE-4A9D-A622-24EF3B0D69B5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB5003FB-30CE-4A9D-A622-24EF3B0D69B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>